<commit_message>
[JN] major update 2.0 on 2024-02-02
</commit_message>
<xml_diff>
--- a/config/watchlist_template.xlsx
+++ b/config/watchlist_template.xlsx
@@ -15,7 +15,7 @@
     <sheet name="watchlist" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">watchlist!$A$1:$AB$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">watchlist!$A$1:$AF$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>symbol</t>
   </si>
@@ -111,6 +111,18 @@
   </si>
   <si>
     <t>sma5_flag</t>
+  </si>
+  <si>
+    <t>ema5_flag</t>
+  </si>
+  <si>
+    <t>csp_bullish_candle</t>
+  </si>
+  <si>
+    <t>is_first_buy_yn</t>
+  </si>
+  <si>
+    <t>volume_inconsistency_alert</t>
   </si>
 </sst>
 </file>
@@ -167,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -186,6 +198,13 @@
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,9 +485,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB1"/>
+  <dimension ref="A1:AF1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -477,14 +496,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="6" width="11.5546875" style="6"/>
-    <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="10" width="26.77734375" customWidth="1"/>
-    <col min="11" max="12" width="11.5546875" style="7"/>
-    <col min="13" max="17" width="10.77734375" style="6" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="7" width="11.5546875" style="6"/>
+    <col min="8" max="9" width="11.5546875" style="8"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="11" max="13" width="26.77734375" customWidth="1"/>
+    <col min="14" max="15" width="11.5546875" style="7"/>
+    <col min="16" max="20" width="10.77734375" style="6" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,85 +514,109 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB1"/>
-  <conditionalFormatting sqref="R1:AB1048576">
+  <autoFilter ref="A1:AF1"/>
+  <conditionalFormatting sqref="U1:AE1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF1:AF1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
[JN] updated on 3/15/2024
</commit_message>
<xml_diff>
--- a/config/watchlist_template.xlsx
+++ b/config/watchlist_template.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9330"/>
   </bookViews>
   <sheets>
     <sheet name="watchlist" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">watchlist!$A$1:$AF$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">watchlist!$A$1:$AJ$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>symbol</t>
   </si>
@@ -123,6 +123,18 @@
   </si>
   <si>
     <t>volume_inconsistency_alert</t>
+  </si>
+  <si>
+    <t>ha_real2_flag</t>
+  </si>
+  <si>
+    <t>today_zone</t>
+  </si>
+  <si>
+    <t>advisory</t>
+  </si>
+  <si>
+    <t>rising_flag</t>
   </si>
 </sst>
 </file>
@@ -179,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -205,11 +217,43 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -485,7 +529,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF1"/>
+  <dimension ref="A1:AJ1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
@@ -494,17 +538,20 @@
       <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="7" width="11.5546875" style="6"/>
-    <col min="8" max="9" width="11.5546875" style="8"/>
+    <col min="5" max="7" width="11.5703125" style="6"/>
+    <col min="8" max="9" width="11.5703125" style="8"/>
     <col min="10" max="10" width="21" customWidth="1"/>
-    <col min="11" max="13" width="26.77734375" customWidth="1"/>
-    <col min="14" max="15" width="11.5546875" style="7"/>
-    <col min="16" max="20" width="10.77734375" style="6" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="13" width="26.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="26.7109375" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="26.7109375" customWidth="1"/>
+    <col min="16" max="17" width="11.5703125" style="7"/>
+    <col min="18" max="22" width="10.7109375" style="6" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="11.5703125" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,68 +591,80 @@
       <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AF1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AF1"/>
-  <conditionalFormatting sqref="U1:AE1048576">
-    <cfRule type="colorScale" priority="2">
+  <autoFilter ref="A1:AJ1"/>
+  <conditionalFormatting sqref="W1:AI1048576">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -616,8 +675,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF1:AF1048576">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="AJ1:AJ1048576">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -628,6 +687,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="O1:O1048576">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="green">
+      <formula>NOT(ISERROR(SEARCH("green",O1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="blue">
+      <formula>NOT(ISERROR(SEARCH("blue",O1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="purple">
+      <formula>NOT(ISERROR(SEARCH("purple",O1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="red">
+      <formula>NOT(ISERROR(SEARCH("red",O1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>